<commit_message>
Documtent Changes And Veranstalter Register
</commit_message>
<xml_diff>
--- a/Documents/Daily_Scrum.xlsx
+++ b/Documents/Daily_Scrum.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C486CE-9460-4E9F-A51D-1614E1F41A6F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B51BF0-0A35-49DA-92BF-AEAEACD86931}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="66">
   <si>
     <t>Datum</t>
   </si>
@@ -142,9 +142,6 @@
     <t>Anw.</t>
   </si>
   <si>
-    <t>Data Analysis</t>
-  </si>
-  <si>
     <t>Webservice Register, Login</t>
   </si>
   <si>
@@ -185,6 +182,42 @@
   </si>
   <si>
     <t>GUI Grobstrukturen in den einzelnen Fragments erstellen</t>
+  </si>
+  <si>
+    <t>Product Owner</t>
+  </si>
+  <si>
+    <t>Veranstalter App Login &amp; Register</t>
+  </si>
+  <si>
+    <t>Veranstalter App Login &amp; Registrieren</t>
+  </si>
+  <si>
+    <t>Qualtitätsverbesserung des Codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glassfish wollte nicht mehr laufen </t>
+  </si>
+  <si>
+    <t>Glassfish neu Herunterladen</t>
+  </si>
+  <si>
+    <t>Emails zum Registrieren verschicken</t>
+  </si>
+  <si>
+    <t>Tabellen durch Textboxen ersetzen</t>
+  </si>
+  <si>
+    <t>geladene Daten in Gui einfügen</t>
+  </si>
+  <si>
+    <t>App abgestürzt</t>
+  </si>
+  <si>
+    <t>Problem: bei der Übergabe der Parameter zur DB</t>
+  </si>
+  <si>
+    <t>Teilnehmer App: Verbessern ListView Layout</t>
   </si>
 </sst>
 </file>
@@ -243,7 +276,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -300,11 +333,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -345,45 +387,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -418,32 +421,66 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
-    <dxf>
-      <font>
-        <color rgb="FF009900"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9799"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <strike val="0"/>
@@ -462,389 +499,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF009900"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1132,13 +786,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD114"/>
+  <dimension ref="A1:AD308"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="G43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T28" sqref="T28"/>
+      <selection pane="bottomRight" activeCell="W74" sqref="W74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1167,53 +821,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="26" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="26" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="26" t="s">
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="26" t="s">
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="48"/>
+      <c r="AB1" s="48"/>
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="48"/>
     </row>
     <row r="2" spans="1:30" s="14" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="30"/>
+      <c r="A2" s="46"/>
       <c r="B2" s="12" t="s">
         <v>39</v>
       </c>
@@ -1274,15 +928,15 @@
       <c r="U2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="V2" s="24"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
-      <c r="AB2" s="25"/>
-      <c r="AC2" s="25"/>
-      <c r="AD2" s="25"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="41"/>
+      <c r="X2" s="41"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
+      <c r="AA2" s="50"/>
+      <c r="AB2" s="50"/>
+      <c r="AC2" s="50"/>
+      <c r="AD2" s="50"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="10">
@@ -1319,6 +973,10 @@
       <c r="T3" t="s">
         <v>10</v>
       </c>
+      <c r="W3" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="X3" s="51"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="10">
@@ -1360,6 +1018,8 @@
       <c r="T4" t="s">
         <v>10</v>
       </c>
+      <c r="W4" s="52"/>
+      <c r="X4" s="52"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="10">
@@ -1396,6 +1056,8 @@
       <c r="T5" t="s">
         <v>10</v>
       </c>
+      <c r="W5" s="52"/>
+      <c r="X5" s="52"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="10">
@@ -1431,6 +1093,10 @@
       <c r="T6" t="s">
         <v>10</v>
       </c>
+      <c r="W6" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="X6" s="52"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="10">
@@ -1472,38 +1138,40 @@
       <c r="T7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
-      <c r="X8" s="18"/>
-      <c r="Y8" s="18"/>
-      <c r="Z8" s="18"/>
-      <c r="AA8" s="18"/>
-      <c r="AB8" s="18"/>
-      <c r="AC8" s="18"/>
-      <c r="AD8" s="18"/>
+      <c r="W7" s="52"/>
+      <c r="X7" s="52"/>
+    </row>
+    <row r="8" spans="1:30" s="39" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="38"/>
+      <c r="S8" s="38"/>
+      <c r="T8" s="38"/>
+      <c r="U8" s="38"/>
+      <c r="V8" s="38"/>
+      <c r="W8" s="38"/>
+      <c r="X8" s="38"/>
+      <c r="Y8" s="38"/>
+      <c r="Z8" s="38"/>
+      <c r="AA8" s="38"/>
+      <c r="AB8" s="38"/>
+      <c r="AC8" s="38"/>
+      <c r="AD8" s="38"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="10">
@@ -1531,14 +1199,18 @@
         <v>24</v>
       </c>
       <c r="P9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>24</v>
       </c>
       <c r="T9" t="s">
-        <v>49</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="W9" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="X9" s="52"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="10">
@@ -1569,8 +1241,10 @@
         <v>24</v>
       </c>
       <c r="T10" t="s">
-        <v>49</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="W10" s="52"/>
+      <c r="X10" s="52"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10">
@@ -1607,8 +1281,10 @@
         <v>24</v>
       </c>
       <c r="T11" t="s">
-        <v>49</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="W11" s="52"/>
+      <c r="X11" s="52"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="10">
@@ -1639,14 +1315,16 @@
         <v>24</v>
       </c>
       <c r="P12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R12" s="4" t="s">
         <v>24</v>
       </c>
       <c r="T12" t="s">
-        <v>49</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="W12" s="52"/>
+      <c r="X12" s="52"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="10">
@@ -1674,63 +1352,65 @@
         <v>24</v>
       </c>
       <c r="P13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="T13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="18"/>
-      <c r="AA14" s="18"/>
-      <c r="AB14" s="18"/>
-      <c r="AC14" s="18"/>
-      <c r="AD14" s="18"/>
-    </row>
-    <row r="15" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="33">
+        <v>48</v>
+      </c>
+      <c r="W13" s="52"/>
+      <c r="X13" s="52"/>
+    </row>
+    <row r="14" spans="1:30" s="39" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="38"/>
+      <c r="S14" s="38"/>
+      <c r="T14" s="38"/>
+      <c r="U14" s="38"/>
+      <c r="V14" s="38"/>
+      <c r="W14" s="38"/>
+      <c r="X14" s="38"/>
+      <c r="Y14" s="38"/>
+      <c r="Z14" s="38"/>
+      <c r="AA14" s="38"/>
+      <c r="AB14" s="38"/>
+      <c r="AC14" s="38"/>
+      <c r="AD14" s="38"/>
+    </row>
+    <row r="15" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="20">
         <v>43178</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="37"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="37"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="37"/>
-      <c r="Q15" s="39"/>
-      <c r="R15" s="37"/>
-      <c r="U15" s="39"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="24"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="24"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="24"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="24"/>
+      <c r="U15" s="26"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="10">
@@ -1758,7 +1438,7 @@
         <v>24</v>
       </c>
       <c r="P16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q16" s="6" t="s">
         <v>29</v>
@@ -1767,8 +1447,12 @@
         <v>24</v>
       </c>
       <c r="T16" t="s">
-        <v>51</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="W16" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="X16" s="52"/>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="10">
@@ -1796,7 +1480,7 @@
         <v>24</v>
       </c>
       <c r="P17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>29</v>
@@ -1805,8 +1489,10 @@
         <v>24</v>
       </c>
       <c r="T17" t="s">
-        <v>51</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="W17" s="52"/>
+      <c r="X17" s="52"/>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="10">
@@ -1831,7 +1517,7 @@
         <v>24</v>
       </c>
       <c r="P18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>29</v>
@@ -1840,8 +1526,12 @@
         <v>24</v>
       </c>
       <c r="T18" t="s">
-        <v>51</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="W18" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="X18" s="52"/>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="10">
@@ -1872,7 +1562,7 @@
         <v>24</v>
       </c>
       <c r="P19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q19" s="6" t="s">
         <v>29</v>
@@ -1881,72 +1571,74 @@
         <v>24</v>
       </c>
       <c r="T19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" s="21" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="20"/>
-      <c r="U20" s="20"/>
-      <c r="V20" s="20"/>
-      <c r="W20" s="20"/>
-      <c r="X20" s="20"/>
-      <c r="Y20" s="20"/>
-      <c r="Z20" s="20"/>
-      <c r="AA20" s="20"/>
-      <c r="AB20" s="20"/>
-      <c r="AC20" s="20"/>
-      <c r="AD20" s="20"/>
-    </row>
-    <row r="21" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="33">
+        <v>50</v>
+      </c>
+      <c r="W19" s="52"/>
+      <c r="X19" s="52"/>
+    </row>
+    <row r="20" spans="1:30" s="37" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="36"/>
+      <c r="R20" s="36"/>
+      <c r="S20" s="36"/>
+      <c r="T20" s="36"/>
+      <c r="U20" s="36"/>
+      <c r="V20" s="36"/>
+      <c r="W20" s="36"/>
+      <c r="X20" s="36"/>
+      <c r="Y20" s="36"/>
+      <c r="Z20" s="36"/>
+      <c r="AA20" s="36"/>
+      <c r="AB20" s="36"/>
+      <c r="AC20" s="36"/>
+      <c r="AD20" s="36"/>
+    </row>
+    <row r="21" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="20">
         <v>43192</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="37"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="37"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="37"/>
-      <c r="Q21" s="39"/>
-      <c r="R21" s="37"/>
-      <c r="U21" s="39"/>
-    </row>
-    <row r="22" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="33">
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="24"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="24"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="24"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="24"/>
+      <c r="U21" s="26"/>
+    </row>
+    <row r="22" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="20">
         <v>43193</v>
       </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="37"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="37"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="37"/>
-      <c r="Q22" s="39"/>
-      <c r="R22" s="37"/>
-      <c r="U22" s="39"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="28"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="24"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="24"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="24"/>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="24"/>
+      <c r="U22" s="26"/>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="10">
@@ -1977,7 +1669,7 @@
         <v>24</v>
       </c>
       <c r="P23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R23" s="4" t="s">
         <v>24</v>
@@ -1985,6 +1677,10 @@
       <c r="T23" t="s">
         <v>21</v>
       </c>
+      <c r="W23" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="X23" s="52"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="10">
@@ -2006,7 +1702,7 @@
         <v>24</v>
       </c>
       <c r="P24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R24" s="4" t="s">
         <v>24</v>
@@ -2014,6 +1710,8 @@
       <c r="T24" t="s">
         <v>21</v>
       </c>
+      <c r="W24" s="52"/>
+      <c r="X24" s="52"/>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="10">
@@ -2038,7 +1736,7 @@
         <v>24</v>
       </c>
       <c r="P25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R25" s="4" t="s">
         <v>24</v>
@@ -2046,38 +1744,40 @@
       <c r="T25" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
-      <c r="T26" s="18"/>
-      <c r="U26" s="18"/>
-      <c r="V26" s="18"/>
-      <c r="W26" s="18"/>
-      <c r="X26" s="18"/>
-      <c r="Y26" s="18"/>
-      <c r="Z26" s="18"/>
-      <c r="AA26" s="18"/>
-      <c r="AB26" s="18"/>
-      <c r="AC26" s="18"/>
-      <c r="AD26" s="18"/>
+      <c r="W25" s="52"/>
+      <c r="X25" s="52"/>
+    </row>
+    <row r="26" spans="1:30" s="39" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="38"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="38"/>
+      <c r="R26" s="38"/>
+      <c r="S26" s="38"/>
+      <c r="T26" s="38"/>
+      <c r="U26" s="38"/>
+      <c r="V26" s="38"/>
+      <c r="W26" s="38"/>
+      <c r="X26" s="38"/>
+      <c r="Y26" s="38"/>
+      <c r="Z26" s="38"/>
+      <c r="AA26" s="38"/>
+      <c r="AB26" s="38"/>
+      <c r="AC26" s="38"/>
+      <c r="AD26" s="38"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="10">
@@ -2105,7 +1805,7 @@
         <v>24</v>
       </c>
       <c r="P27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R27" s="4" t="s">
         <v>24</v>
@@ -2113,6 +1813,10 @@
       <c r="T27" t="s">
         <v>21</v>
       </c>
+      <c r="W27" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="X27" s="52"/>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="10">
@@ -2140,7 +1844,7 @@
         <v>24</v>
       </c>
       <c r="P28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R28" s="4" t="s">
         <v>24</v>
@@ -2148,6 +1852,8 @@
       <c r="T28" t="s">
         <v>21</v>
       </c>
+      <c r="W28" s="52"/>
+      <c r="X28" s="52"/>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="10">
@@ -2169,7 +1875,7 @@
         <v>32</v>
       </c>
       <c r="H29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>24</v>
@@ -2184,7 +1890,7 @@
         <v>24</v>
       </c>
       <c r="P29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R29" s="4" t="s">
         <v>24</v>
@@ -2192,6 +1898,8 @@
       <c r="T29" t="s">
         <v>21</v>
       </c>
+      <c r="W29" s="52"/>
+      <c r="X29" s="52"/>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="10">
@@ -2207,7 +1915,7 @@
         <v>24</v>
       </c>
       <c r="H30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>24</v>
@@ -2219,7 +1927,7 @@
         <v>24</v>
       </c>
       <c r="P30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R30" s="4" t="s">
         <v>24</v>
@@ -2227,6 +1935,8 @@
       <c r="T30" t="s">
         <v>21</v>
       </c>
+      <c r="W30" s="52"/>
+      <c r="X30" s="52"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="10">
@@ -2245,7 +1955,7 @@
         <v>24</v>
       </c>
       <c r="H31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>24</v>
@@ -2260,7 +1970,7 @@
         <v>24</v>
       </c>
       <c r="P31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R31" s="4" t="s">
         <v>24</v>
@@ -2268,38 +1978,40 @@
       <c r="T31" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="32" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
-      <c r="U32" s="18"/>
-      <c r="V32" s="18"/>
-      <c r="W32" s="18"/>
-      <c r="X32" s="18"/>
-      <c r="Y32" s="18"/>
-      <c r="Z32" s="18"/>
-      <c r="AA32" s="18"/>
-      <c r="AB32" s="18"/>
-      <c r="AC32" s="18"/>
-      <c r="AD32" s="18"/>
+      <c r="W31" s="52"/>
+      <c r="X31" s="52"/>
+    </row>
+    <row r="32" spans="1:30" s="39" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="38"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="38"/>
+      <c r="L32" s="38"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="38"/>
+      <c r="P32" s="38"/>
+      <c r="Q32" s="38"/>
+      <c r="R32" s="38"/>
+      <c r="S32" s="38"/>
+      <c r="T32" s="38"/>
+      <c r="U32" s="38"/>
+      <c r="V32" s="38"/>
+      <c r="W32" s="38"/>
+      <c r="X32" s="38"/>
+      <c r="Y32" s="38"/>
+      <c r="Z32" s="38"/>
+      <c r="AA32" s="38"/>
+      <c r="AB32" s="38"/>
+      <c r="AC32" s="38"/>
+      <c r="AD32" s="38"/>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="10">
@@ -2315,19 +2027,19 @@
         <v>24</v>
       </c>
       <c r="H33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R33" s="4" t="s">
         <v>24</v>
@@ -2335,6 +2047,10 @@
       <c r="T33" t="s">
         <v>21</v>
       </c>
+      <c r="W33" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="X33" s="52"/>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="10">
@@ -2350,19 +2066,19 @@
         <v>24</v>
       </c>
       <c r="H34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R34" s="4" t="s">
         <v>24</v>
@@ -2370,6 +2086,8 @@
       <c r="T34" t="s">
         <v>21</v>
       </c>
+      <c r="W34" s="52"/>
+      <c r="X34" s="52"/>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="10">
@@ -2385,19 +2103,19 @@
         <v>24</v>
       </c>
       <c r="H35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R35" s="4" t="s">
         <v>24</v>
@@ -2405,6 +2123,10 @@
       <c r="T35" t="s">
         <v>21</v>
       </c>
+      <c r="W35" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="X35" s="52"/>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="10">
@@ -2420,19 +2142,19 @@
         <v>24</v>
       </c>
       <c r="H36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R36" s="4" t="s">
         <v>24</v>
@@ -2440,6 +2162,8 @@
       <c r="T36" t="s">
         <v>21</v>
       </c>
+      <c r="W36" s="52"/>
+      <c r="X36" s="52"/>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="10">
@@ -2455,19 +2179,19 @@
         <v>24</v>
       </c>
       <c r="H37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R37" s="4" t="s">
         <v>24</v>
@@ -2475,8 +2199,10 @@
       <c r="T37" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="38" spans="1:30" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+      <c r="W37" s="52"/>
+      <c r="X37" s="52"/>
+    </row>
+    <row r="38" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="39" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="10">
         <v>43213</v>
@@ -2497,7 +2223,7 @@
         <v>24</v>
       </c>
       <c r="L39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N39" s="4" t="s">
         <v>24</v>
@@ -2511,6 +2237,10 @@
       <c r="T39" t="s">
         <v>21</v>
       </c>
+      <c r="W39" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="X39" s="52"/>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="10">
@@ -2532,7 +2262,7 @@
         <v>24</v>
       </c>
       <c r="L40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N40" s="4" t="s">
         <v>24</v>
@@ -2546,6 +2276,8 @@
       <c r="T40" t="s">
         <v>21</v>
       </c>
+      <c r="W40" s="52"/>
+      <c r="X40" s="52"/>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="10">
@@ -2567,7 +2299,7 @@
         <v>24</v>
       </c>
       <c r="L41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>24</v>
@@ -2581,6 +2313,8 @@
       <c r="T41" t="s">
         <v>21</v>
       </c>
+      <c r="W41" s="52"/>
+      <c r="X41" s="52"/>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="10">
@@ -2590,7 +2324,7 @@
         <v>24</v>
       </c>
       <c r="D42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>24</v>
@@ -2602,7 +2336,7 @@
         <v>24</v>
       </c>
       <c r="L42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N42" s="4" t="s">
         <v>24</v>
@@ -2616,6 +2350,8 @@
       <c r="T42" t="s">
         <v>21</v>
       </c>
+      <c r="W42" s="52"/>
+      <c r="X42" s="52"/>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="10">
@@ -2625,7 +2361,7 @@
         <v>24</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>24</v>
@@ -2637,7 +2373,7 @@
         <v>24</v>
       </c>
       <c r="L43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>24</v>
@@ -2651,57 +2387,59 @@
       <c r="T43" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="44" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="45" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="42">
+      <c r="W43" s="52"/>
+      <c r="X43" s="52"/>
+    </row>
+    <row r="44" spans="1:30" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="45" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="29">
         <v>43250</v>
       </c>
-      <c r="B45" s="40"/>
-      <c r="C45" s="41"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="37"/>
-      <c r="I45" s="43"/>
-      <c r="J45" s="37"/>
-      <c r="M45" s="43"/>
-      <c r="N45" s="37"/>
-      <c r="Q45" s="43"/>
-      <c r="R45" s="37"/>
-      <c r="U45" s="43"/>
-    </row>
-    <row r="46" spans="1:30" s="47" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="44">
+      <c r="B45" s="27"/>
+      <c r="C45" s="28"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="24"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="24"/>
+      <c r="M45" s="30"/>
+      <c r="N45" s="24"/>
+      <c r="Q45" s="30"/>
+      <c r="R45" s="24"/>
+      <c r="U45" s="30"/>
+    </row>
+    <row r="46" spans="1:30" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="31">
         <v>43221</v>
       </c>
-      <c r="B46" s="45"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="46"/>
-      <c r="H46" s="46"/>
-      <c r="I46" s="46"/>
-      <c r="J46" s="45"/>
-      <c r="K46" s="46"/>
-      <c r="L46" s="46"/>
-      <c r="M46" s="46"/>
-      <c r="N46" s="45"/>
-      <c r="O46" s="46"/>
-      <c r="P46" s="46"/>
-      <c r="Q46" s="46"/>
-      <c r="R46" s="45"/>
-      <c r="S46" s="46"/>
-      <c r="T46" s="46"/>
-      <c r="U46" s="46"/>
-      <c r="V46" s="46"/>
-      <c r="W46" s="46"/>
-      <c r="X46" s="46"/>
-      <c r="Y46" s="46"/>
-      <c r="Z46" s="46"/>
-      <c r="AA46" s="46"/>
-      <c r="AB46" s="46"/>
-      <c r="AC46" s="46"/>
-      <c r="AD46" s="46"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="32"/>
+      <c r="K46" s="33"/>
+      <c r="L46" s="33"/>
+      <c r="M46" s="33"/>
+      <c r="N46" s="32"/>
+      <c r="O46" s="33"/>
+      <c r="P46" s="33"/>
+      <c r="Q46" s="33"/>
+      <c r="R46" s="32"/>
+      <c r="S46" s="33"/>
+      <c r="T46" s="33"/>
+      <c r="U46" s="33"/>
+      <c r="V46" s="33"/>
+      <c r="W46" s="33"/>
+      <c r="X46" s="33"/>
+      <c r="Y46" s="33"/>
+      <c r="Z46" s="33"/>
+      <c r="AA46" s="33"/>
+      <c r="AB46" s="33"/>
+      <c r="AC46" s="33"/>
+      <c r="AD46" s="33"/>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="10">
@@ -2711,7 +2449,7 @@
         <v>24</v>
       </c>
       <c r="D47" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>24</v>
@@ -2723,7 +2461,7 @@
         <v>24</v>
       </c>
       <c r="L47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>24</v>
@@ -2737,6 +2475,10 @@
       <c r="T47" t="s">
         <v>21</v>
       </c>
+      <c r="W47" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="X47" s="52"/>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="10">
@@ -2746,7 +2488,7 @@
         <v>24</v>
       </c>
       <c r="D48" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>24</v>
@@ -2758,7 +2500,7 @@
         <v>24</v>
       </c>
       <c r="L48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>24</v>
@@ -2772,6 +2514,8 @@
       <c r="T48" t="s">
         <v>21</v>
       </c>
+      <c r="W48" s="52"/>
+      <c r="X48" s="52"/>
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="10">
@@ -2781,7 +2525,7 @@
         <v>24</v>
       </c>
       <c r="D49" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>24</v>
@@ -2793,7 +2537,7 @@
         <v>24</v>
       </c>
       <c r="L49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>24</v>
@@ -2807,38 +2551,40 @@
       <c r="T49" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="50" spans="1:30" s="21" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
-      <c r="M50" s="20"/>
-      <c r="N50" s="20"/>
-      <c r="O50" s="20"/>
-      <c r="P50" s="20"/>
-      <c r="Q50" s="20"/>
-      <c r="R50" s="20"/>
-      <c r="S50" s="20"/>
-      <c r="T50" s="20"/>
-      <c r="U50" s="20"/>
-      <c r="V50" s="20"/>
-      <c r="W50" s="20"/>
-      <c r="X50" s="20"/>
-      <c r="Y50" s="20"/>
-      <c r="Z50" s="20"/>
-      <c r="AA50" s="20"/>
-      <c r="AB50" s="20"/>
-      <c r="AC50" s="20"/>
-      <c r="AD50" s="20"/>
+      <c r="W49" s="52"/>
+      <c r="X49" s="52"/>
+    </row>
+    <row r="50" spans="1:30" s="37" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="36"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="36"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="36"/>
+      <c r="J50" s="36"/>
+      <c r="K50" s="36"/>
+      <c r="L50" s="36"/>
+      <c r="M50" s="36"/>
+      <c r="N50" s="36"/>
+      <c r="O50" s="36"/>
+      <c r="P50" s="36"/>
+      <c r="Q50" s="36"/>
+      <c r="R50" s="36"/>
+      <c r="S50" s="36"/>
+      <c r="T50" s="36"/>
+      <c r="U50" s="36"/>
+      <c r="V50" s="36"/>
+      <c r="W50" s="36"/>
+      <c r="X50" s="36"/>
+      <c r="Y50" s="36"/>
+      <c r="Z50" s="36"/>
+      <c r="AA50" s="36"/>
+      <c r="AB50" s="36"/>
+      <c r="AC50" s="36"/>
+      <c r="AD50" s="36"/>
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="10">
@@ -2848,32 +2594,36 @@
         <v>24</v>
       </c>
       <c r="D51" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H51" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J51" s="17" t="s">
         <v>24</v>
       </c>
       <c r="L51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P51" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R51" s="4" t="s">
         <v>24</v>
       </c>
       <c r="T51" t="s">
-        <v>44</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="W51" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="X51" s="52"/>
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="10">
@@ -2883,32 +2633,34 @@
         <v>24</v>
       </c>
       <c r="D52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J52" s="17" t="s">
         <v>24</v>
       </c>
       <c r="L52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N52" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P52" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R52" s="4" t="s">
         <v>24</v>
       </c>
       <c r="T52" t="s">
-        <v>44</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="W52" s="52"/>
+      <c r="X52" s="52"/>
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="10">
@@ -2918,115 +2670,117 @@
         <v>24</v>
       </c>
       <c r="D53" t="s">
-        <v>46</v>
-      </c>
-      <c r="E53" s="31"/>
+        <v>45</v>
+      </c>
+      <c r="E53" s="18"/>
       <c r="F53" s="4" t="s">
         <v>25</v>
       </c>
       <c r="H53" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L53" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P53" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R53" s="4" t="s">
         <v>25</v>
       </c>
       <c r="T53" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="54" spans="1:30" s="47" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="44">
+        <v>43</v>
+      </c>
+      <c r="W53" s="52"/>
+      <c r="X53" s="52"/>
+    </row>
+    <row r="54" spans="1:30" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="31">
         <v>43230</v>
       </c>
-      <c r="B54" s="46"/>
-      <c r="C54" s="46"/>
-      <c r="D54" s="46"/>
-      <c r="E54" s="46"/>
-      <c r="F54" s="45"/>
-      <c r="G54" s="46"/>
-      <c r="H54" s="46"/>
-      <c r="I54" s="46"/>
-      <c r="J54" s="45"/>
-      <c r="K54" s="46"/>
-      <c r="L54" s="46"/>
-      <c r="M54" s="46"/>
-      <c r="N54" s="45"/>
-      <c r="O54" s="46"/>
-      <c r="P54" s="46"/>
-      <c r="Q54" s="46"/>
-      <c r="R54" s="45"/>
-      <c r="S54" s="46"/>
-      <c r="T54" s="46"/>
-      <c r="U54" s="46"/>
-      <c r="V54" s="46"/>
-      <c r="W54" s="46"/>
-      <c r="X54" s="46"/>
-      <c r="Y54" s="46"/>
-      <c r="Z54" s="46"/>
-      <c r="AA54" s="46"/>
-      <c r="AB54" s="46"/>
-      <c r="AC54" s="46"/>
-      <c r="AD54" s="46"/>
-    </row>
-    <row r="55" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="44">
+      <c r="B54" s="33"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="33"/>
+      <c r="I54" s="33"/>
+      <c r="J54" s="32"/>
+      <c r="K54" s="33"/>
+      <c r="L54" s="33"/>
+      <c r="M54" s="33"/>
+      <c r="N54" s="32"/>
+      <c r="O54" s="33"/>
+      <c r="P54" s="33"/>
+      <c r="Q54" s="33"/>
+      <c r="R54" s="32"/>
+      <c r="S54" s="33"/>
+      <c r="T54" s="33"/>
+      <c r="U54" s="33"/>
+      <c r="V54" s="33"/>
+      <c r="W54" s="33"/>
+      <c r="X54" s="33"/>
+      <c r="Y54" s="33"/>
+      <c r="Z54" s="33"/>
+      <c r="AA54" s="33"/>
+      <c r="AB54" s="33"/>
+      <c r="AC54" s="33"/>
+      <c r="AD54" s="33"/>
+    </row>
+    <row r="55" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="31">
         <v>43231</v>
       </c>
-      <c r="B55" s="40"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="43"/>
-      <c r="E55" s="48"/>
-      <c r="F55" s="37"/>
-      <c r="I55" s="39"/>
-      <c r="M55" s="39"/>
-      <c r="N55" s="37"/>
-      <c r="Q55" s="39"/>
-      <c r="R55" s="37"/>
-      <c r="U55" s="39"/>
-    </row>
-    <row r="56" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="18"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="18"/>
-      <c r="K56" s="18"/>
-      <c r="L56" s="18"/>
-      <c r="M56" s="18"/>
-      <c r="N56" s="18"/>
-      <c r="O56" s="18"/>
-      <c r="P56" s="18"/>
-      <c r="Q56" s="18"/>
-      <c r="R56" s="18"/>
-      <c r="S56" s="18"/>
-      <c r="T56" s="18"/>
-      <c r="U56" s="18"/>
-      <c r="V56" s="18"/>
-      <c r="W56" s="18"/>
-      <c r="X56" s="18"/>
-      <c r="Y56" s="18"/>
-      <c r="Z56" s="18"/>
-      <c r="AA56" s="18"/>
-      <c r="AB56" s="18"/>
-      <c r="AC56" s="18"/>
-      <c r="AD56" s="18"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="24"/>
+      <c r="I55" s="26"/>
+      <c r="M55" s="26"/>
+      <c r="N55" s="24"/>
+      <c r="Q55" s="26"/>
+      <c r="R55" s="24"/>
+      <c r="U55" s="26"/>
+    </row>
+    <row r="56" spans="1:30" s="39" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="38"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="38"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="38"/>
+      <c r="J56" s="38"/>
+      <c r="K56" s="38"/>
+      <c r="L56" s="38"/>
+      <c r="M56" s="38"/>
+      <c r="N56" s="38"/>
+      <c r="O56" s="38"/>
+      <c r="P56" s="38"/>
+      <c r="Q56" s="38"/>
+      <c r="R56" s="38"/>
+      <c r="S56" s="38"/>
+      <c r="T56" s="38"/>
+      <c r="U56" s="38"/>
+      <c r="V56" s="38"/>
+      <c r="W56" s="38"/>
+      <c r="X56" s="38"/>
+      <c r="Y56" s="38"/>
+      <c r="Z56" s="38"/>
+      <c r="AA56" s="38"/>
+      <c r="AB56" s="38"/>
+      <c r="AC56" s="38"/>
+      <c r="AD56" s="38"/>
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="10">
@@ -3035,327 +2789,1120 @@
       <c r="B57" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
+      <c r="D57" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E57" s="18"/>
       <c r="F57" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J57" s="32" t="s">
-        <v>24</v>
+      <c r="H57" t="s">
+        <v>57</v>
+      </c>
+      <c r="J57" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="L57" t="s">
+        <v>60</v>
       </c>
       <c r="N57" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="P57" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q57" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="R57" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="T57" t="s">
+        <v>65</v>
+      </c>
+      <c r="W57" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="X57" s="52"/>
     </row>
     <row r="58" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="10">
         <v>43235</v>
       </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="N58" s="4"/>
-      <c r="R58" s="4"/>
+      <c r="B58" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E58" s="18"/>
+      <c r="F58" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H58" t="s">
+        <v>57</v>
+      </c>
+      <c r="J58" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="L58" t="s">
+        <v>60</v>
+      </c>
+      <c r="N58" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P58" t="s">
+        <v>61</v>
+      </c>
+      <c r="R58" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T58" t="s">
+        <v>65</v>
+      </c>
+      <c r="W58" s="52"/>
+      <c r="X58" s="52"/>
     </row>
     <row r="59" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="10">
         <v>43236</v>
       </c>
-      <c r="D59" s="5"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="N59" s="4"/>
-      <c r="R59" s="4"/>
+      <c r="B59" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E59" s="53"/>
+      <c r="F59" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H59" t="s">
+        <v>57</v>
+      </c>
+      <c r="J59" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="L59" t="s">
+        <v>59</v>
+      </c>
+      <c r="M59" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="N59" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P59" t="s">
+        <v>62</v>
+      </c>
+      <c r="R59" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T59" t="s">
+        <v>65</v>
+      </c>
+      <c r="W59" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="X59" s="52"/>
     </row>
     <row r="60" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="10">
         <v>43237</v>
       </c>
-      <c r="D60" s="4"/>
-      <c r="E60" s="5"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="18"/>
       <c r="F60" s="5"/>
       <c r="N60" s="4"/>
       <c r="R60" s="4"/>
+      <c r="W60" s="52"/>
+      <c r="X60" s="52"/>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="10">
         <v>43238</v>
       </c>
       <c r="B61" s="4"/>
-      <c r="E61" s="5"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="18"/>
       <c r="F61" s="5"/>
       <c r="N61" s="4"/>
       <c r="R61" s="4"/>
-    </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="10"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="N62" s="4"/>
-    </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="10">
+      <c r="W61" s="52"/>
+      <c r="X61" s="52"/>
+    </row>
+    <row r="62" spans="1:30" s="37" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="36"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="36"/>
+      <c r="F62" s="36"/>
+      <c r="G62" s="36"/>
+      <c r="H62" s="36"/>
+      <c r="I62" s="36"/>
+      <c r="J62" s="36"/>
+      <c r="K62" s="36"/>
+      <c r="L62" s="36"/>
+      <c r="M62" s="36"/>
+      <c r="N62" s="36"/>
+      <c r="O62" s="36"/>
+      <c r="P62" s="36"/>
+      <c r="Q62" s="36"/>
+      <c r="R62" s="36"/>
+      <c r="S62" s="36"/>
+      <c r="T62" s="36"/>
+      <c r="U62" s="36"/>
+      <c r="V62" s="36"/>
+      <c r="W62" s="36"/>
+      <c r="X62" s="36"/>
+      <c r="Y62" s="36"/>
+      <c r="Z62" s="36"/>
+      <c r="AA62" s="36"/>
+      <c r="AB62" s="36"/>
+      <c r="AC62" s="36"/>
+      <c r="AD62" s="36"/>
+    </row>
+    <row r="63" spans="1:30" s="29" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="29">
         <v>43241</v>
       </c>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="N63" s="4"/>
-    </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="10">
+    </row>
+    <row r="64" spans="1:30" s="29" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="29">
         <v>43242</v>
       </c>
-      <c r="B64" s="4"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
-      <c r="N64" s="4"/>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="10">
         <v>43243</v>
       </c>
-      <c r="E65" s="5"/>
+      <c r="D65" s="54"/>
+      <c r="E65" s="18"/>
       <c r="F65" s="5"/>
       <c r="N65" s="4"/>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="W65" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="X65" s="52"/>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="10">
         <v>43244</v>
       </c>
-      <c r="E66" s="4"/>
+      <c r="D66" s="54"/>
+      <c r="E66" s="53"/>
       <c r="F66" s="4"/>
       <c r="N66" s="4"/>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="W66" s="52"/>
+      <c r="X66" s="52"/>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="10">
         <v>43245</v>
       </c>
-      <c r="E67" s="5"/>
+      <c r="D67" s="54"/>
+      <c r="E67" s="18"/>
       <c r="F67" s="5"/>
       <c r="N67" s="4"/>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="10"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="W67" s="52"/>
+      <c r="X67" s="52"/>
+    </row>
+    <row r="68" spans="1:24" s="37" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="36"/>
+      <c r="B68" s="36"/>
+      <c r="C68" s="36"/>
+      <c r="D68" s="36"/>
+      <c r="E68" s="36"/>
+      <c r="F68" s="36"/>
+      <c r="G68" s="36"/>
+      <c r="H68" s="36"/>
+      <c r="I68" s="36"/>
+      <c r="J68" s="36"/>
+      <c r="K68" s="36"/>
+      <c r="L68" s="36"/>
+      <c r="M68" s="36"/>
+      <c r="N68" s="36"/>
+      <c r="O68" s="36"/>
+      <c r="P68" s="36"/>
+      <c r="Q68" s="36"/>
+      <c r="R68" s="36"/>
+      <c r="S68" s="36"/>
+      <c r="T68" s="36"/>
+      <c r="U68" s="36"/>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="10">
         <v>43248</v>
       </c>
-      <c r="E69" s="4"/>
+      <c r="D69" s="54"/>
+      <c r="E69" s="53"/>
       <c r="F69" s="4"/>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="W69" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="X69" s="52"/>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="10">
         <v>43249</v>
       </c>
-      <c r="E70" s="5"/>
+      <c r="D70" s="54"/>
+      <c r="E70" s="18"/>
       <c r="F70" s="5"/>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="W70" s="52"/>
+      <c r="X70" s="52"/>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="10">
         <v>43250</v>
       </c>
       <c r="B71" s="4"/>
-      <c r="E71" s="5"/>
+      <c r="D71" s="54"/>
+      <c r="E71" s="18"/>
       <c r="F71" s="5"/>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="W71" s="52"/>
+      <c r="X71" s="52"/>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="10">
         <v>43251</v>
       </c>
-      <c r="E72" s="5"/>
+      <c r="D72" s="54"/>
+      <c r="E72" s="18"/>
       <c r="F72" s="5"/>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="W72" s="52"/>
+      <c r="X72" s="52"/>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="10">
         <v>43252</v>
       </c>
-      <c r="E73" s="4"/>
+      <c r="D73" s="54"/>
+      <c r="E73" s="53"/>
       <c r="F73" s="4"/>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="E74" s="5"/>
+      <c r="W73" s="52"/>
+      <c r="X73" s="52"/>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="D74" s="54"/>
+      <c r="E74" s="18"/>
       <c r="F74" s="5"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="B75" s="4"/>
-      <c r="E75" s="5"/>
+      <c r="D75" s="54"/>
+      <c r="E75" s="18"/>
       <c r="F75" s="5"/>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="E76" s="5"/>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="D76" s="54"/>
+      <c r="E76" s="18"/>
       <c r="F76" s="5"/>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="E77" s="4"/>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="D77" s="54"/>
+      <c r="E77" s="53"/>
       <c r="F77" s="4"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="E78" s="5"/>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="D78" s="54"/>
+      <c r="E78" s="18"/>
       <c r="F78" s="5"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="B79" s="4"/>
-      <c r="E79" s="5"/>
+      <c r="D79" s="54"/>
+      <c r="E79" s="18"/>
       <c r="F79" s="5"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="E80" s="5"/>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="D80" s="54"/>
+      <c r="E80" s="18"/>
       <c r="F80" s="5"/>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E81" s="4"/>
+      <c r="D81" s="54"/>
+      <c r="E81" s="53"/>
       <c r="F81" s="4"/>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E82" s="5"/>
+      <c r="D82" s="54"/>
+      <c r="E82" s="18"/>
       <c r="F82" s="5"/>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B83" s="4"/>
-      <c r="E83" s="5"/>
+      <c r="D83" s="54"/>
+      <c r="E83" s="18"/>
       <c r="F83" s="5"/>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E84" s="5"/>
+      <c r="D84" s="54"/>
+      <c r="E84" s="18"/>
       <c r="F84" s="5"/>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E85" s="4"/>
+      <c r="D85" s="54"/>
+      <c r="E85" s="53"/>
       <c r="F85" s="4"/>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E86" s="5"/>
+      <c r="D86" s="54"/>
+      <c r="E86" s="18"/>
       <c r="F86" s="5"/>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B87" s="4"/>
-      <c r="E87" s="5"/>
+      <c r="D87" s="54"/>
+      <c r="E87" s="18"/>
       <c r="F87" s="5"/>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E88" s="5"/>
+      <c r="D88" s="54"/>
+      <c r="E88" s="18"/>
       <c r="F88" s="5"/>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E89" s="4"/>
+      <c r="D89" s="54"/>
+      <c r="E89" s="53"/>
       <c r="F89" s="4"/>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E90" s="5"/>
+      <c r="D90" s="54"/>
+      <c r="E90" s="18"/>
       <c r="F90" s="5"/>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B91" s="4"/>
-      <c r="E91" s="5"/>
+      <c r="D91" s="54"/>
+      <c r="E91" s="18"/>
       <c r="F91" s="5"/>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E92" s="5"/>
+      <c r="D92" s="54"/>
+      <c r="E92" s="18"/>
       <c r="F92" s="5"/>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E93" s="4"/>
+      <c r="D93" s="54"/>
+      <c r="E93" s="53"/>
       <c r="F93" s="4"/>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E94" s="5"/>
+      <c r="D94" s="54"/>
+      <c r="E94" s="18"/>
       <c r="F94" s="5"/>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B95" s="4"/>
-      <c r="E95" s="5"/>
+      <c r="D95" s="54"/>
+      <c r="E95" s="18"/>
       <c r="F95" s="5"/>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E96" s="5"/>
+      <c r="D96" s="54"/>
+      <c r="E96" s="18"/>
       <c r="F96" s="5"/>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E97" s="4"/>
+      <c r="D97" s="54"/>
+      <c r="E97" s="53"/>
       <c r="F97" s="4"/>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E98" s="5"/>
+      <c r="D98" s="54"/>
+      <c r="E98" s="18"/>
       <c r="F98" s="5"/>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B99" s="4"/>
-      <c r="E99" s="5"/>
+      <c r="D99" s="54"/>
+      <c r="E99" s="18"/>
       <c r="F99" s="5"/>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E100" s="5"/>
+      <c r="D100" s="54"/>
+      <c r="E100" s="18"/>
       <c r="F100" s="5"/>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E101" s="4"/>
+      <c r="D101" s="54"/>
+      <c r="E101" s="53"/>
       <c r="F101" s="4"/>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E102" s="5"/>
+      <c r="D102" s="54"/>
+      <c r="E102" s="18"/>
       <c r="F102" s="5"/>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B103" s="4"/>
-      <c r="E103" s="5"/>
+      <c r="D103" s="54"/>
+      <c r="E103" s="18"/>
       <c r="F103" s="5"/>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E104" s="5"/>
+      <c r="D104" s="54"/>
+      <c r="E104" s="18"/>
       <c r="F104" s="5"/>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E105" s="4"/>
+      <c r="D105" s="54"/>
+      <c r="E105" s="53"/>
       <c r="F105" s="4"/>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E106" s="5"/>
+      <c r="D106" s="54"/>
+      <c r="E106" s="18"/>
       <c r="F106" s="5"/>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E107" s="5"/>
+      <c r="D107" s="54"/>
+      <c r="E107" s="18"/>
       <c r="F107" s="5"/>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E108" s="5"/>
+      <c r="D108" s="54"/>
+      <c r="E108" s="18"/>
       <c r="F108" s="5"/>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E109" s="4"/>
+      <c r="D109" s="54"/>
+      <c r="E109" s="53"/>
       <c r="F109" s="4"/>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E110" s="5"/>
+      <c r="D110" s="54"/>
+      <c r="E110" s="18"/>
       <c r="F110" s="5"/>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E111" s="5"/>
+      <c r="D111" s="54"/>
+      <c r="E111" s="18"/>
       <c r="F111" s="5"/>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E112" s="5"/>
+      <c r="D112" s="54"/>
+      <c r="E112" s="18"/>
       <c r="F112" s="5"/>
     </row>
-    <row r="113" spans="5:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E113" s="4"/>
+    <row r="113" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D113" s="54"/>
+      <c r="E113" s="53"/>
       <c r="F113" s="4"/>
     </row>
-    <row r="114" spans="5:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E114" s="5"/>
+    <row r="114" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D114" s="54"/>
+      <c r="E114" s="18"/>
       <c r="F114" s="5"/>
     </row>
+    <row r="115" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D115" s="54"/>
+    </row>
+    <row r="116" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D116" s="54"/>
+    </row>
+    <row r="117" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D117" s="54"/>
+    </row>
+    <row r="118" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D118" s="54"/>
+    </row>
+    <row r="119" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D119" s="54"/>
+    </row>
+    <row r="120" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D120" s="54"/>
+    </row>
+    <row r="121" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D121" s="54"/>
+    </row>
+    <row r="122" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D122" s="54"/>
+    </row>
+    <row r="123" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D123" s="54"/>
+    </row>
+    <row r="124" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D124" s="54"/>
+    </row>
+    <row r="125" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D125" s="54"/>
+    </row>
+    <row r="126" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D126" s="54"/>
+    </row>
+    <row r="127" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D127" s="54"/>
+    </row>
+    <row r="128" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D128" s="54"/>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D129" s="54"/>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D130" s="54"/>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D131" s="54"/>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D132" s="54"/>
+    </row>
+    <row r="133" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D133" s="54"/>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D134" s="54"/>
+    </row>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D135" s="54"/>
+    </row>
+    <row r="136" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D136" s="54"/>
+    </row>
+    <row r="137" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D137" s="54"/>
+    </row>
+    <row r="138" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D138" s="54"/>
+    </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D139" s="54"/>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D140" s="54"/>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D141" s="54"/>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D142" s="54"/>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D143" s="54"/>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D144" s="54"/>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D145" s="54"/>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D146" s="54"/>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D147" s="54"/>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D148" s="54"/>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D149" s="54"/>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D150" s="54"/>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D151" s="54"/>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D152" s="54"/>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D153" s="54"/>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D154" s="54"/>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D155" s="54"/>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D156" s="54"/>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D157" s="54"/>
+    </row>
+    <row r="158" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D158" s="54"/>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D159" s="54"/>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D160" s="54"/>
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D161" s="54"/>
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D162" s="54"/>
+    </row>
+    <row r="163" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D163" s="54"/>
+    </row>
+    <row r="164" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D164" s="54"/>
+    </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D165" s="54"/>
+    </row>
+    <row r="166" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D166" s="54"/>
+    </row>
+    <row r="167" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D167" s="54"/>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D168" s="54"/>
+    </row>
+    <row r="169" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D169" s="54"/>
+    </row>
+    <row r="170" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D170" s="54"/>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D171" s="54"/>
+    </row>
+    <row r="172" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D172" s="54"/>
+    </row>
+    <row r="173" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D173" s="54"/>
+    </row>
+    <row r="174" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D174" s="54"/>
+    </row>
+    <row r="175" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D175" s="54"/>
+    </row>
+    <row r="176" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D176" s="54"/>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D177" s="54"/>
+    </row>
+    <row r="178" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D178" s="54"/>
+    </row>
+    <row r="179" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D179" s="54"/>
+    </row>
+    <row r="180" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D180" s="54"/>
+    </row>
+    <row r="181" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D181" s="54"/>
+    </row>
+    <row r="182" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D182" s="54"/>
+    </row>
+    <row r="183" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D183" s="54"/>
+    </row>
+    <row r="184" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D184" s="54"/>
+    </row>
+    <row r="185" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D185" s="54"/>
+    </row>
+    <row r="186" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D186" s="54"/>
+    </row>
+    <row r="187" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D187" s="54"/>
+    </row>
+    <row r="188" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D188" s="54"/>
+    </row>
+    <row r="189" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D189" s="54"/>
+    </row>
+    <row r="190" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D190" s="54"/>
+    </row>
+    <row r="191" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D191" s="54"/>
+    </row>
+    <row r="192" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D192" s="54"/>
+    </row>
+    <row r="193" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D193" s="54"/>
+    </row>
+    <row r="194" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D194" s="54"/>
+    </row>
+    <row r="195" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D195" s="54"/>
+    </row>
+    <row r="196" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D196" s="54"/>
+    </row>
+    <row r="197" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D197" s="54"/>
+    </row>
+    <row r="198" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D198" s="54"/>
+    </row>
+    <row r="199" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D199" s="54"/>
+    </row>
+    <row r="200" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D200" s="54"/>
+    </row>
+    <row r="201" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D201" s="54"/>
+    </row>
+    <row r="202" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D202" s="54"/>
+    </row>
+    <row r="203" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D203" s="54"/>
+    </row>
+    <row r="204" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D204" s="54"/>
+    </row>
+    <row r="205" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D205" s="54"/>
+    </row>
+    <row r="206" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D206" s="54"/>
+    </row>
+    <row r="207" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D207" s="54"/>
+    </row>
+    <row r="208" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D208" s="54"/>
+    </row>
+    <row r="209" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D209" s="54"/>
+    </row>
+    <row r="210" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D210" s="54"/>
+    </row>
+    <row r="211" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D211" s="54"/>
+    </row>
+    <row r="212" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D212" s="54"/>
+    </row>
+    <row r="213" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D213" s="54"/>
+    </row>
+    <row r="214" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D214" s="54"/>
+    </row>
+    <row r="215" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D215" s="54"/>
+    </row>
+    <row r="216" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D216" s="54"/>
+    </row>
+    <row r="217" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D217" s="54"/>
+    </row>
+    <row r="218" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D218" s="54"/>
+    </row>
+    <row r="219" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D219" s="54"/>
+    </row>
+    <row r="220" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D220" s="54"/>
+    </row>
+    <row r="221" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D221" s="54"/>
+    </row>
+    <row r="222" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D222" s="54"/>
+    </row>
+    <row r="223" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D223" s="54"/>
+    </row>
+    <row r="224" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D224" s="54"/>
+    </row>
+    <row r="225" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D225" s="54"/>
+    </row>
+    <row r="226" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D226" s="54"/>
+    </row>
+    <row r="227" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D227" s="54"/>
+    </row>
+    <row r="228" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D228" s="54"/>
+    </row>
+    <row r="229" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D229" s="54"/>
+    </row>
+    <row r="230" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D230" s="54"/>
+    </row>
+    <row r="231" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D231" s="54"/>
+    </row>
+    <row r="232" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D232" s="54"/>
+    </row>
+    <row r="233" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D233" s="54"/>
+    </row>
+    <row r="234" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D234" s="54"/>
+    </row>
+    <row r="235" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D235" s="54"/>
+    </row>
+    <row r="236" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D236" s="54"/>
+    </row>
+    <row r="237" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D237" s="54"/>
+    </row>
+    <row r="238" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D238" s="54"/>
+    </row>
+    <row r="239" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D239" s="54"/>
+    </row>
+    <row r="240" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D240" s="54"/>
+    </row>
+    <row r="241" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D241" s="54"/>
+    </row>
+    <row r="242" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D242" s="54"/>
+    </row>
+    <row r="243" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D243" s="54"/>
+    </row>
+    <row r="244" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D244" s="54"/>
+    </row>
+    <row r="245" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D245" s="54"/>
+    </row>
+    <row r="246" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D246" s="54"/>
+    </row>
+    <row r="247" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D247" s="54"/>
+    </row>
+    <row r="248" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D248" s="54"/>
+    </row>
+    <row r="249" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D249" s="54"/>
+    </row>
+    <row r="250" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D250" s="54"/>
+    </row>
+    <row r="251" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D251" s="54"/>
+    </row>
+    <row r="252" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D252" s="54"/>
+    </row>
+    <row r="253" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D253" s="54"/>
+    </row>
+    <row r="254" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D254" s="54"/>
+    </row>
+    <row r="255" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D255" s="54"/>
+    </row>
+    <row r="256" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D256" s="54"/>
+    </row>
+    <row r="257" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D257" s="54"/>
+    </row>
+    <row r="258" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D258" s="54"/>
+    </row>
+    <row r="259" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D259" s="54"/>
+    </row>
+    <row r="260" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D260" s="54"/>
+    </row>
+    <row r="261" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D261" s="54"/>
+    </row>
+    <row r="262" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D262" s="54"/>
+    </row>
+    <row r="263" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D263" s="54"/>
+    </row>
+    <row r="264" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D264" s="54"/>
+    </row>
+    <row r="265" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D265" s="54"/>
+    </row>
+    <row r="266" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D266" s="54"/>
+    </row>
+    <row r="267" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D267" s="54"/>
+    </row>
+    <row r="268" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D268" s="54"/>
+    </row>
+    <row r="269" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D269" s="54"/>
+    </row>
+    <row r="270" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D270" s="54"/>
+    </row>
+    <row r="271" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D271" s="54"/>
+    </row>
+    <row r="272" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D272" s="54"/>
+    </row>
+    <row r="273" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D273" s="54"/>
+    </row>
+    <row r="274" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D274" s="54"/>
+    </row>
+    <row r="275" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D275" s="54"/>
+    </row>
+    <row r="276" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D276" s="54"/>
+    </row>
+    <row r="277" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D277" s="54"/>
+    </row>
+    <row r="278" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D278" s="54"/>
+    </row>
+    <row r="279" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D279" s="54"/>
+    </row>
+    <row r="280" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D280" s="54"/>
+    </row>
+    <row r="281" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D281" s="54"/>
+    </row>
+    <row r="282" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D282" s="54"/>
+    </row>
+    <row r="283" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D283" s="54"/>
+    </row>
+    <row r="284" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D284" s="54"/>
+    </row>
+    <row r="285" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D285" s="54"/>
+    </row>
+    <row r="286" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D286" s="54"/>
+    </row>
+    <row r="287" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D287" s="54"/>
+    </row>
+    <row r="288" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D288" s="54"/>
+    </row>
+    <row r="289" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D289" s="54"/>
+    </row>
+    <row r="290" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D290" s="54"/>
+    </row>
+    <row r="291" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D291" s="54"/>
+    </row>
+    <row r="292" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D292" s="54"/>
+    </row>
+    <row r="293" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D293" s="54"/>
+    </row>
+    <row r="294" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D294" s="54"/>
+    </row>
+    <row r="295" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D295" s="54"/>
+    </row>
+    <row r="296" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D296" s="54"/>
+    </row>
+    <row r="297" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D297" s="54"/>
+    </row>
+    <row r="298" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D298" s="54"/>
+    </row>
+    <row r="299" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D299" s="54"/>
+    </row>
+    <row r="300" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D300" s="54"/>
+    </row>
+    <row r="301" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D301" s="54"/>
+    </row>
+    <row r="302" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D302" s="54"/>
+    </row>
+    <row r="303" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D303" s="54"/>
+    </row>
+    <row r="304" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D304" s="54"/>
+    </row>
+    <row r="305" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D305" s="54"/>
+    </row>
+    <row r="306" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D306" s="54"/>
+    </row>
+    <row r="307" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D307" s="54"/>
+    </row>
+    <row r="308" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D308" s="54"/>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="34">
+    <mergeCell ref="A62:XFD62"/>
+    <mergeCell ref="A68:XFD68"/>
+    <mergeCell ref="W59:X61"/>
+    <mergeCell ref="W69:X73"/>
+    <mergeCell ref="W65:X67"/>
+    <mergeCell ref="W33:X34"/>
+    <mergeCell ref="W27:X31"/>
+    <mergeCell ref="W23:X25"/>
+    <mergeCell ref="W18:X19"/>
+    <mergeCell ref="W57:X58"/>
+    <mergeCell ref="W51:X53"/>
+    <mergeCell ref="W47:X49"/>
+    <mergeCell ref="W39:X43"/>
+    <mergeCell ref="W35:X37"/>
+    <mergeCell ref="W1:X2"/>
+    <mergeCell ref="W3:X5"/>
+    <mergeCell ref="W16:X17"/>
+    <mergeCell ref="W9:X13"/>
+    <mergeCell ref="W6:X7"/>
     <mergeCell ref="A44:XFD44"/>
     <mergeCell ref="A50:XFD50"/>
     <mergeCell ref="A56:XFD56"/>
-    <mergeCell ref="V1:AD2"/>
     <mergeCell ref="A8:XFD8"/>
     <mergeCell ref="A14:XFD14"/>
     <mergeCell ref="R1:U1"/>
@@ -3369,12 +3916,12 @@
     <mergeCell ref="A26:XFD26"/>
     <mergeCell ref="A32:XFD32"/>
   </mergeCells>
-  <conditionalFormatting sqref="B1:B55 F1:F55 J1:J55 N1:N55 R1:R55 R57:R1048576 N57:N1048576 J57:J1048576 F57:F1048576 B57:B1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+  <conditionalFormatting sqref="B1:B55 F1:F55 J1:J55 N1:N55 R1:R55 B65:B67 F65:F67 J65:J67 N65:N67 R65:R67 R69:R1048576 N69:N1048576 J69:J1048576 F69:F1048576 B69:B1048576 J57:J61 N57:N61 R57:R61 B57:B61 F57:F61">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"nein"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>